<commit_message>
forgot to update this file since last change
</commit_message>
<xml_diff>
--- a/learningcurve vs randai.xlsx
+++ b/learningcurve vs randai.xlsx
@@ -15,6 +15,7 @@
     <sheet name="learningcurve" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -596,7 +597,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t> Curve</a:t>
+              <a:t> Curve Against Random AI</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -640,7 +641,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Learn AI Winrate</c:v>
+            <c:v>Learn AI Win</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -661,64 +662,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>1500</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="16">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9500</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -730,67 +731,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>116</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>147</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>153</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>159</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>174</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>161</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>185</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>175</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>184</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>173</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>179</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>171</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>172</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>178</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>169</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>174</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>185</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>171</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>194</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -805,7 +806,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Rand AI Winrate</c:v>
+            <c:v>Rand AI Win</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -826,64 +827,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>1500</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="16">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9500</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -895,67 +896,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>114</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>124</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>102</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>84</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>84</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>76</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>79</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>70</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>60</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>57</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>60</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>53</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>66</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>59</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>54</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>64</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>55</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -970,7 +971,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Tie Rate</c:v>
+            <c:v>Tie</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -991,64 +992,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>1500</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="16">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6500</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9500</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1060,67 +1061,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>270</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>246</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>266</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>251</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>257</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>242</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>263</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>260</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>246</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>246</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>267</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>264</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>269</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>275</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>256</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>272</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>272</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>251</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>274</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>265</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1874,14 +1875,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>109537</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>414337</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2209,7 +2210,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="A1:L22"/>
+      <selection sqref="A1:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,293 +2220,293 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="C1">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="D1">
-        <v>270</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="B2">
-        <v>130</v>
+        <v>29</v>
       </c>
       <c r="C2">
-        <v>124</v>
+        <v>22</v>
       </c>
       <c r="D2">
-        <v>246</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="B3">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>266</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1500</v>
+        <v>300</v>
       </c>
       <c r="B4">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="C4">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="D4">
-        <v>251</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="B5">
-        <v>153</v>
+        <v>39</v>
       </c>
       <c r="C5">
-        <v>91</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>256</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="B6">
-        <v>159</v>
+        <v>41</v>
       </c>
       <c r="C6">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>257</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="B7">
-        <v>174</v>
+        <v>50</v>
       </c>
       <c r="C7">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>242</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3500</v>
+        <v>700</v>
       </c>
       <c r="B8">
-        <v>161</v>
+        <v>38</v>
       </c>
       <c r="C8">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>263</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4000</v>
+        <v>800</v>
       </c>
       <c r="B9">
-        <v>185</v>
+        <v>41</v>
       </c>
       <c r="C9">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <v>260</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4500</v>
+        <v>900</v>
       </c>
       <c r="B10">
-        <v>175</v>
+        <v>49</v>
       </c>
       <c r="C10">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>246</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="B11">
-        <v>184</v>
+        <v>39</v>
       </c>
       <c r="C11">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>246</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5500</v>
+        <v>1100</v>
       </c>
       <c r="B12">
-        <v>173</v>
+        <v>47</v>
       </c>
       <c r="C12">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>267</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6000</v>
+        <v>1200</v>
       </c>
       <c r="B13">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="C13">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>264</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>6500</v>
+        <v>1300</v>
       </c>
       <c r="B14">
-        <v>171</v>
+        <v>43</v>
       </c>
       <c r="C14">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>269</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>7000</v>
+        <v>1400</v>
       </c>
       <c r="B15">
-        <v>172</v>
+        <v>52</v>
       </c>
       <c r="C15">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>275</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>7500</v>
+        <v>1500</v>
       </c>
       <c r="B16">
-        <v>178</v>
+        <v>46</v>
       </c>
       <c r="C16">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>256</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>8000</v>
+        <v>1600</v>
       </c>
       <c r="B17">
-        <v>169</v>
+        <v>52</v>
       </c>
       <c r="C17">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>272</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>8500</v>
+        <v>1700</v>
       </c>
       <c r="B18">
-        <v>174</v>
+        <v>47</v>
       </c>
       <c r="C18">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>272</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>9000</v>
+        <v>1800</v>
       </c>
       <c r="B19">
-        <v>185</v>
+        <v>44</v>
       </c>
       <c r="C19">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>251</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>9500</v>
+        <v>1900</v>
       </c>
       <c r="B20">
-        <v>171</v>
+        <v>50</v>
       </c>
       <c r="C20">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>274</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="B21">
-        <v>194</v>
+        <v>46</v>
       </c>
       <c r="C21">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>265</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>